<commit_message>
Current controlled voltage source representation
</commit_message>
<xml_diff>
--- a/PV Farm/Text/Txt creator(hourly).xlsx
+++ b/PV Farm/Text/Txt creator(hourly).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>#1</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>1/B_int</t>
+  </si>
+  <si>
+    <t>windspeed</t>
+  </si>
+  <si>
+    <t>irradiance</t>
   </si>
 </sst>
 </file>
@@ -86,13 +92,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -396,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,7 +417,7 @@
     <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -425,8 +434,16 @@
         <v>5</v>
       </c>
       <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="P1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +457,14 @@
       <c r="J2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -455,8 +478,14 @@
       <c r="J3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -481,8 +510,20 @@
       <c r="K4" s="1">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>17.181999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3600</v>
       </c>
@@ -507,8 +548,20 @@
       <c r="K5" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>3600</v>
+      </c>
+      <c r="N5">
+        <v>17.54</v>
+      </c>
+      <c r="P5">
+        <v>3600</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>7200</v>
       </c>
@@ -533,8 +586,20 @@
       <c r="K6" s="1">
         <v>198.86857008578599</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>7200</v>
+      </c>
+      <c r="N6">
+        <v>17.815999999999999</v>
+      </c>
+      <c r="P6">
+        <v>7200</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>10800</v>
       </c>
@@ -559,8 +624,20 @@
       <c r="K7" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>10800</v>
+      </c>
+      <c r="N7">
+        <v>17.844999999999999</v>
+      </c>
+      <c r="P7">
+        <v>10800</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>14400</v>
       </c>
@@ -585,8 +662,20 @@
       <c r="K8" s="1">
         <v>1320</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M8">
+        <v>14400</v>
+      </c>
+      <c r="N8">
+        <v>17.774999999999999</v>
+      </c>
+      <c r="P8">
+        <v>14400</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>18000</v>
       </c>
@@ -611,8 +700,20 @@
       <c r="K9" s="1">
         <v>1320</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M9">
+        <v>18000</v>
+      </c>
+      <c r="N9">
+        <v>17.71</v>
+      </c>
+      <c r="P9">
+        <v>18000</v>
+      </c>
+      <c r="Q9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>21600</v>
       </c>
@@ -637,8 +738,20 @@
       <c r="K10" s="1">
         <v>1980</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M10">
+        <v>21600</v>
+      </c>
+      <c r="N10">
+        <v>17.623000000000001</v>
+      </c>
+      <c r="P10">
+        <v>21600</v>
+      </c>
+      <c r="Q10">
+        <v>21.558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>25200</v>
       </c>
@@ -663,8 +776,20 @@
       <c r="K11" s="1">
         <v>2872.5594919159098</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>25200</v>
+      </c>
+      <c r="N11">
+        <v>17.687999999999999</v>
+      </c>
+      <c r="P11">
+        <v>25200</v>
+      </c>
+      <c r="Q11">
+        <v>103.485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>28800</v>
       </c>
@@ -689,8 +814,20 @@
       <c r="K12" s="1">
         <v>5470.91846466064</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>28800</v>
+      </c>
+      <c r="N12">
+        <v>17.702999999999999</v>
+      </c>
+      <c r="P12">
+        <v>28800</v>
+      </c>
+      <c r="Q12">
+        <v>236.392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>32400</v>
       </c>
@@ -715,8 +852,20 @@
       <c r="K13" s="1">
         <v>7001.0007315658904</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>32400</v>
+      </c>
+      <c r="N13">
+        <v>17.757000000000001</v>
+      </c>
+      <c r="P13">
+        <v>32400</v>
+      </c>
+      <c r="Q13">
+        <v>311.10300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>36000</v>
       </c>
@@ -741,8 +890,20 @@
       <c r="K14" s="1">
         <v>6435</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>36000</v>
+      </c>
+      <c r="N14">
+        <v>17.794</v>
+      </c>
+      <c r="P14">
+        <v>36000</v>
+      </c>
+      <c r="Q14">
+        <v>287.56799999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>39600</v>
       </c>
@@ -767,8 +928,20 @@
       <c r="K15" s="1">
         <v>3960</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>39600</v>
+      </c>
+      <c r="N15">
+        <v>17.707999999999998</v>
+      </c>
+      <c r="P15">
+        <v>39600</v>
+      </c>
+      <c r="Q15">
+        <v>290.94200000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43200</v>
       </c>
@@ -793,8 +966,20 @@
       <c r="K16" s="1">
         <v>2310</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>43200</v>
+      </c>
+      <c r="N16">
+        <v>17.300999999999998</v>
+      </c>
+      <c r="P16">
+        <v>43200</v>
+      </c>
+      <c r="Q16">
+        <v>316.97899999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>46800</v>
       </c>
@@ -819,8 +1004,20 @@
       <c r="K17" s="1">
         <v>3443.1732263250001</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>46800</v>
+      </c>
+      <c r="N17">
+        <v>16.866</v>
+      </c>
+      <c r="P17">
+        <v>46800</v>
+      </c>
+      <c r="Q17">
+        <v>306.72899999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>50400</v>
       </c>
@@ -845,8 +1042,20 @@
       <c r="K18" s="1">
         <v>3960</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>50400</v>
+      </c>
+      <c r="N18">
+        <v>16.175999999999998</v>
+      </c>
+      <c r="P18">
+        <v>50400</v>
+      </c>
+      <c r="Q18">
+        <v>201.322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>54000</v>
       </c>
@@ -871,8 +1080,20 @@
       <c r="K19" s="1">
         <v>6435</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>54000</v>
+      </c>
+      <c r="N19">
+        <v>15.555999999999999</v>
+      </c>
+      <c r="P19">
+        <v>54000</v>
+      </c>
+      <c r="Q19">
+        <v>157.17699999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>57600</v>
       </c>
@@ -897,8 +1118,20 @@
       <c r="K20" s="1">
         <v>495</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>57600</v>
+      </c>
+      <c r="N20">
+        <v>15.239000000000001</v>
+      </c>
+      <c r="P20">
+        <v>57600</v>
+      </c>
+      <c r="Q20">
+        <v>74.778000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>61200</v>
       </c>
@@ -923,8 +1156,20 @@
       <c r="K21" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>61200</v>
+      </c>
+      <c r="N21">
+        <v>14.932</v>
+      </c>
+      <c r="P21">
+        <v>61200</v>
+      </c>
+      <c r="Q21">
+        <v>5.6230000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>64800</v>
       </c>
@@ -949,8 +1194,20 @@
       <c r="K22" s="1">
         <v>20.518085360000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <v>64800</v>
+      </c>
+      <c r="N22">
+        <v>14.414999999999999</v>
+      </c>
+      <c r="P22">
+        <v>64800</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>68400</v>
       </c>
@@ -975,8 +1232,20 @@
       <c r="K23" s="1">
         <v>17.952000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M23">
+        <v>68400</v>
+      </c>
+      <c r="N23">
+        <v>13.882999999999999</v>
+      </c>
+      <c r="P23">
+        <v>68400</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>72000</v>
       </c>
@@ -1001,8 +1270,20 @@
       <c r="K24" s="1">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>72000</v>
+      </c>
+      <c r="N24">
+        <v>13.446999999999999</v>
+      </c>
+      <c r="P24">
+        <v>72000</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>75600</v>
       </c>
@@ -1027,8 +1308,20 @@
       <c r="K25" s="1">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <v>75600</v>
+      </c>
+      <c r="N25">
+        <v>13.548</v>
+      </c>
+      <c r="P25">
+        <v>75600</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>79200</v>
       </c>
@@ -1053,8 +1346,20 @@
       <c r="K26" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M26">
+        <v>79200</v>
+      </c>
+      <c r="N26">
+        <v>13.382</v>
+      </c>
+      <c r="P26">
+        <v>79200</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>82800</v>
       </c>
@@ -1079,17 +1384,43 @@
       <c r="K27" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M27">
+        <v>82800</v>
+      </c>
+      <c r="N27">
+        <v>12.885999999999999</v>
+      </c>
+      <c r="P27">
+        <v>82800</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
+      <c r="M28">
+        <v>86400</v>
+      </c>
+      <c r="N28">
+        <v>12.471</v>
+      </c>
+      <c r="P28">
+        <v>86400</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>